<commit_message>
Minor bug fixes, added an example inside the excel sheets for reference
</commit_message>
<xml_diff>
--- a/RFQ_template_ht.xlsx
+++ b/RFQ_template_ht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saggarwal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saggarwal\PythonProjects\email_app_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833A4C3A-BFDD-4F9D-9CA1-F1CB9991CC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11496E67-056E-4E9C-BF4C-483A04804C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25380" yWindow="2985" windowWidth="25875" windowHeight="11475" xr2:uid="{F50D261B-B61D-42C3-8F5B-DD738D71A0AE}"/>
+    <workbookView xWindow="-28920" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{F50D261B-B61D-42C3-8F5B-DD738D71A0AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Price</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Currency Code</t>
   </si>
   <si>
-    <t>Shipping Charge</t>
-  </si>
-  <si>
-    <t>Freight</t>
-  </si>
-  <si>
     <t>NRE (non recording pricing)</t>
   </si>
   <si>
@@ -68,27 +62,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Item Description</t>
-  </si>
-  <si>
-    <t>ITAR or Not</t>
-  </si>
-  <si>
-    <t>DPAS rating</t>
-  </si>
-  <si>
-    <t>Need Date</t>
-  </si>
-  <si>
-    <t>Other Charges</t>
-  </si>
-  <si>
-    <t>Rev</t>
-  </si>
-  <si>
-    <t>Certification required</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -108,6 +81,24 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Example Part</t>
+  </si>
+  <si>
+    <t>Example Part Description</t>
+  </si>
+  <si>
+    <t>US Dollar</t>
+  </si>
+  <si>
+    <t>If Any Comments</t>
+  </si>
+  <si>
+    <t>Heat Treat to T6</t>
+  </si>
+  <si>
+    <t>10 Days</t>
   </si>
 </sst>
 </file>
@@ -157,14 +148,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -197,33 +198,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B042E3F6-FD39-4A82-B93C-3F4DB8072C3B}" name="Table1" displayName="Table1" ref="A1:X3" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:X3" xr:uid="{B042E3F6-FD39-4A82-B93C-3F4DB8072C3B}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B042E3F6-FD39-4A82-B93C-3F4DB8072C3B}" name="Table1" displayName="Table1" ref="A1:O2" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:O2" xr:uid="{B042E3F6-FD39-4A82-B93C-3F4DB8072C3B}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{58160B28-F146-4990-8C3F-39FF3E1AF171}" name="Part Number"/>
     <tableColumn id="24" xr3:uid="{47F83571-546D-41B7-BC3D-81944AD14B59}" name="Description"/>
     <tableColumn id="19" xr3:uid="{C1EFC295-4EFF-434A-B0B6-401010D3A360}" name="Qty"/>
     <tableColumn id="23" xr3:uid="{3AB6C6E2-269E-4A4B-A224-34AABC13A939}" name="Thickness"/>
     <tableColumn id="22" xr3:uid="{DB8CC10B-0418-4C49-9CF1-DF5CB2F5EC84}" name="Part Width"/>
     <tableColumn id="20" xr3:uid="{9DF15D92-09AA-4563-9B2F-8EFCC39C3A29}" name="Part Length"/>
-    <tableColumn id="21" xr3:uid="{B04F18CB-D731-4795-969F-802A754D0869}" name="Process"/>
+    <tableColumn id="21" xr3:uid="{B04F18CB-D731-4795-969F-802A754D0869}" name="Process" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{DCB31E8F-936F-468D-BF95-18F7212CC885}" name="Price"/>
     <tableColumn id="3" xr3:uid="{17BD2836-FBE6-4D99-856D-DFA92CE2FA36}" name="ShippingCharge"/>
     <tableColumn id="4" xr3:uid="{E19DE358-BB4F-484A-B9DB-911EEF0BF929}" name="LeadTime"/>
-    <tableColumn id="5" xr3:uid="{154C5B5C-F2B8-47E7-A1D7-0A06F95BB4E8}" name="GoodUntil (MM/DD/YYYY)"/>
+    <tableColumn id="5" xr3:uid="{154C5B5C-F2B8-47E7-A1D7-0A06F95BB4E8}" name="GoodUntil (MM/DD/YYYY)" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{490A78C4-4B25-4831-843B-62F177A82053}" name="Currency Code"/>
-    <tableColumn id="7" xr3:uid="{896BF048-E270-44F6-BE46-11593C8110A6}" name="Shipping Charge"/>
-    <tableColumn id="8" xr3:uid="{1CF9FA65-65A8-4CCC-AA46-42B9F7C415F4}" name="Freight"/>
     <tableColumn id="9" xr3:uid="{84187FEF-8D69-47E2-9634-8F5E0BB3CD11}" name="NRE (non recording pricing)"/>
     <tableColumn id="10" xr3:uid="{6F61A08B-DE3C-4186-9791-D6A0E880EA96}" name="MOQ"/>
     <tableColumn id="11" xr3:uid="{63CC04AF-4292-4AA8-AFBD-241779405936}" name="Comments"/>
-    <tableColumn id="12" xr3:uid="{F8B1103A-D0EC-4383-8C7C-FE0DC4FE022E}" name="Item Description"/>
-    <tableColumn id="13" xr3:uid="{3BCEA43F-127B-44B7-BBE5-C9349F2AF4FE}" name="ITAR or Not"/>
-    <tableColumn id="14" xr3:uid="{51E26066-24FB-4AA0-BA5F-14AF6D1787C7}" name="Certification required"/>
-    <tableColumn id="15" xr3:uid="{401FE082-3C2D-4AA1-B6B7-7BC0BDFA4ECB}" name="DPAS rating"/>
-    <tableColumn id="16" xr3:uid="{011AC7C6-732C-4567-A03F-44BA88BAF9B5}" name="Need Date"/>
-    <tableColumn id="17" xr3:uid="{D73AE4EA-331F-4832-81BD-A2BC3E2EF7F6}" name="Other Charges"/>
-    <tableColumn id="18" xr3:uid="{F624593F-9ACA-4723-9FFD-2521762A893D}" name="Rev"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -546,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AFFA9B-DB76-4B5E-9778-431DB66031D2}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,40 +557,33 @@
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="33.5703125" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
-    <col min="17" max="17" width="28.42578125" customWidth="1"/>
-    <col min="18" max="18" width="21.85546875" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" customWidth="1"/>
-    <col min="20" max="20" width="27.28515625" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -624,32 +609,52 @@
       <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>15</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>3.5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3">
+        <v>45534</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>